<commit_message>
complete working with sheet
</commit_message>
<xml_diff>
--- a/garbase/items.xlsx
+++ b/garbase/items.xlsx
@@ -470,7 +470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,9 +484,12 @@
           <t>Apple</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>79 BDT</t>
+      <c r="B1" t="n">
+        <v>130</v>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>BDT</t>
         </is>
       </c>
     </row>
@@ -496,9 +499,12 @@
           <t>Mango</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>35 BDT</t>
+      <c r="B2" t="n">
+        <v>43</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>BDT</t>
         </is>
       </c>
     </row>
@@ -508,9 +514,12 @@
           <t>Orange</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>100 BDT</t>
+      <c r="B3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>BDT</t>
         </is>
       </c>
     </row>
@@ -520,9 +529,12 @@
           <t>Banana</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1111 BDT</t>
+      <c r="B4" t="n">
+        <v>1111</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>BDT</t>
         </is>
       </c>
     </row>
@@ -532,9 +544,12 @@
           <t>Pineapple</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>96 BDT</t>
+      <c r="B5" t="n">
+        <v>48</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>BDT</t>
         </is>
       </c>
     </row>

</xml_diff>